<commit_message>
Documentazione + Diario + Media
</commit_message>
<xml_diff>
--- a/Documentazione/Analisi/Analisi Costi.xlsx
+++ b/Documentazione/Analisi/Analisi Costi.xlsx
@@ -34,21 +34,9 @@
     <t>Mouse Logitech M90</t>
   </si>
   <si>
-    <t>Switch ZyXEL 5 porte 10/100Mbps</t>
-  </si>
-  <si>
-    <t>Scheda Ethernet</t>
-  </si>
-  <si>
     <t>Totale:</t>
   </si>
   <si>
-    <t>Server proxy</t>
-  </si>
-  <si>
-    <t>Laptop hp</t>
-  </si>
-  <si>
     <t>Ore</t>
   </si>
   <si>
@@ -68,6 +56,18 @@
   </si>
   <si>
     <t>Cavo Ethernet cat 5e (1.5 metri)</t>
+  </si>
+  <si>
+    <t>Switch ZyXEL 5 porte 10/100Mbps x2</t>
+  </si>
+  <si>
+    <t>Scheda Ethernet 100Mbps</t>
+  </si>
+  <si>
+    <t>Server proxy Squid (Ubuntu 16.04)</t>
+  </si>
+  <si>
+    <t>Laptop hp (W10)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,7 +647,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7">
         <v>19.25</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7">
         <v>26.4</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7">
         <v>500</v>
@@ -671,21 +671,21 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7">
         <v>178</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" s="11">
         <v>60</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C13" s="11">
         <v>9.3000000000000007</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" s="11">
         <v>11.3</v>
@@ -719,21 +719,21 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="4">
         <f>SUM($C$4:$C$14)</f>
         <v>1015.0999999999999</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F15" s="4">
         <f>E13*F13</f>
         <v>10800</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I15" s="4">
         <f>SUM(F15,C15)</f>

</xml_diff>